<commit_message>
revise average and remove unnecessary average in Summary124
</commit_message>
<xml_diff>
--- a/storage/excel/sum124.xlsx
+++ b/storage/excel/sum124.xlsx
@@ -1483,22 +1483,22 @@
         <v>21</v>
       </c>
       <c r="R11" s="40">
-        <v>3.5574</v>
+        <v>0.030974471933338</v>
       </c>
       <c r="S11" s="39">
-        <v>0.58163464231668</v>
+        <v>0.0068479122191713</v>
       </c>
       <c r="T11" s="39">
-        <v>4.2523076923077</v>
+        <v>0.052953164575325</v>
       </c>
       <c r="U11" s="39">
-        <v>0.09888688417306</v>
+        <v>0.0016457306606764</v>
       </c>
       <c r="V11" s="39">
-        <v>3.9048538461538</v>
+        <v>0.041963818254331</v>
       </c>
       <c r="W11" s="39">
-        <v>0.34026076324487</v>
+        <v>0.0042468214399239</v>
       </c>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -1558,22 +1558,22 @@
         <v>25</v>
       </c>
       <c r="R12" s="40">
-        <v>86.631</v>
+        <v>0.73876409792649</v>
       </c>
       <c r="S12" s="39">
-        <v>21.290932677685</v>
+        <v>0.30994441750723</v>
       </c>
       <c r="T12" s="39">
-        <v>136.93230769231</v>
+        <v>2.0428731993907</v>
       </c>
       <c r="U12" s="39">
-        <v>3.8807352800474</v>
+        <v>0.064585360230034</v>
       </c>
       <c r="V12" s="39">
-        <v>111.78165384615</v>
+        <v>1.3908186486586</v>
       </c>
       <c r="W12" s="39">
-        <v>12.585833978866</v>
+        <v>0.18726488886863</v>
       </c>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -1635,22 +1635,22 @@
         <v>29</v>
       </c>
       <c r="R13" s="40">
-        <v>3.1536</v>
+        <v>0.027401020605904</v>
       </c>
       <c r="S13" s="41">
-        <v>0.53514644190699</v>
+        <v>0.0065363390157085</v>
       </c>
       <c r="T13" s="41">
-        <v>4.0406153846154</v>
+        <v>0.057164621745122</v>
       </c>
       <c r="U13" s="41">
-        <v>0.10808566409613</v>
+        <v>0.0017988218849254</v>
       </c>
       <c r="V13" s="41">
-        <v>3.5971076923077</v>
+        <v>0.042282821175513</v>
       </c>
       <c r="W13" s="41">
-        <v>0.32161605300156</v>
+        <v>0.004167580450317</v>
       </c>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
@@ -1759,22 +1759,22 @@
         <v>36</v>
       </c>
       <c r="R15" s="40">
-        <v>490.57906</v>
+        <v>4.3135256908468</v>
       </c>
       <c r="S15" s="41">
-        <v>71.373702221196</v>
+        <v>0.68471867233326</v>
       </c>
       <c r="T15" s="41">
-        <v>632.44</v>
+        <v>9.985659882498</v>
       </c>
       <c r="U15" s="41">
-        <v>19.058722153122</v>
+        <v>0.31718588024084</v>
       </c>
       <c r="V15" s="41">
-        <v>561.50953</v>
+        <v>7.1495927866724</v>
       </c>
       <c r="W15" s="41">
-        <v>45.216212187159</v>
+        <v>0.50095227628705</v>
       </c>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
@@ -1807,22 +1807,22 @@
         <v>36</v>
       </c>
       <c r="R16" s="40">
-        <v>154.0656</v>
+        <v>1.3355304696079</v>
       </c>
       <c r="S16" s="41">
-        <v>27.319504366975</v>
+        <v>0.34583884439391</v>
       </c>
       <c r="T16" s="41">
-        <v>281.16133333333</v>
+        <v>4.0207474287372</v>
       </c>
       <c r="U16" s="41">
-        <v>9.3621296599103</v>
+        <v>0.143824413826</v>
       </c>
       <c r="V16" s="41">
-        <v>217.61346666667</v>
+        <v>2.6781389491726</v>
       </c>
       <c r="W16" s="41">
-        <v>18.340817013442</v>
+        <v>0.24483162910996</v>
       </c>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>

</xml_diff>